<commit_message>
Version two of the simulation script changes from spending a fixed percentage of the portfolio to meeting a fixed annual spending amount (like $100,000).
Several bugs were fixed in both the simulation Version 2 script and the Excel double-checker.

The big remaining bug is that the simulation V2 script won't correctly reduce spending of the survivor.

Changes were made to the data file passed between thew data generator script and the simulation script, so the original simulation script may no longer work.
</commit_message>
<xml_diff>
--- a/Check Cotton Retirement Plan R Model.xlsx
+++ b/Check Cotton Retirement Plan R Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1600" windowWidth="19600" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="80" windowWidth="19600" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>scenario</t>
   </si>
@@ -102,37 +102,13 @@
     <t>Male Death Age</t>
   </si>
   <si>
-    <t>maleDeathAge</t>
-  </si>
-  <si>
-    <t>femaleDeathAge</t>
-  </si>
-  <si>
-    <t>equityAlloc</t>
-  </si>
-  <si>
-    <t>annualSpendPercent</t>
-  </si>
-  <si>
-    <t>annualReturn</t>
-  </si>
-  <si>
-    <t>sigma50yr</t>
-  </si>
-  <si>
-    <t>qLAC</t>
-  </si>
-  <si>
-    <t>vcSSclaimAge</t>
-  </si>
-  <si>
-    <t>dcSSclaimAge</t>
-  </si>
-  <si>
     <t>inflation</t>
   </si>
   <si>
     <t>Household SS Benefit</t>
+  </si>
+  <si>
+    <t>Initial Portfolio Value</t>
   </si>
 </sst>
 </file>
@@ -144,7 +120,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +184,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +392,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -465,6 +448,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="181">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -976,15 +960,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X89"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="1" customWidth="1"/>
@@ -993,213 +978,130 @@
     <col min="14" max="14" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13">
         <v>1000</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="13">
         <v>95</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2">
-        <v>95</v>
-      </c>
-      <c r="J2">
-        <v>68</v>
-      </c>
-      <c r="K2">
-        <v>0.8</v>
-      </c>
-      <c r="L2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="M2">
-        <v>0.6</v>
-      </c>
-      <c r="N2">
-        <v>0.217258248494763</v>
-      </c>
-      <c r="O2">
-        <v>0.13039999999999999</v>
-      </c>
-      <c r="P2">
-        <v>75000</v>
-      </c>
-      <c r="Q2">
-        <v>66</v>
-      </c>
-      <c r="R2">
-        <v>24540</v>
-      </c>
-      <c r="S2">
-        <v>65</v>
-      </c>
-      <c r="T2">
-        <v>27823</v>
-      </c>
-      <c r="U2">
-        <v>0.05</v>
-      </c>
-      <c r="V2">
-        <v>0.05</v>
-      </c>
-      <c r="W2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="X2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="D2" s="13"/>
+      <c r="K2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="13">
         <v>68</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="13">
         <v>0.8</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="13">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="13">
         <v>0.6</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="13">
         <v>0.217258248494763</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="13">
         <v>0.13039999999999999</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="13">
         <v>75000</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>66</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="13">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>24540</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="13">
-        <v>24540</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>65</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="13">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>27823</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="13">
-        <v>36888</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1207,7 +1109,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1215,9 +1117,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>2.5000000000000001E-2</v>
@@ -1229,7 +1131,12 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="B18" s="4"/>
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4000000</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="B19" s="4"/>
@@ -1256,8 +1163,8 @@
         <v>12</v>
       </c>
       <c r="E22" s="19">
-        <f>1000000-$B$9-($B$6*(1000000-$B$9))</f>
-        <v>370000</v>
+        <f>$B$18-$B$9-($B$6*($B$18-$B$9))</f>
+        <v>1570000</v>
       </c>
       <c r="F22" s="20" t="s">
         <v>16</v>
@@ -1266,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="I22" s="16" t="s">
         <v>7</v>
@@ -1297,7 +1204,7 @@
       </c>
       <c r="E23" s="1">
         <f>(E22-K23)*(1+D23)</f>
-        <v>364603.20953307068</v>
+        <v>1547100.1053160026</v>
       </c>
       <c r="F23" s="1">
         <f>IF(AND(C23&lt;&gt;" ",C23&gt;$B$10),$B$11*(1+$B$16)^(A23-1),0)</f>
@@ -1311,17 +1218,17 @@
         <f>IF(AND(B23&lt;&gt;" ",C23&lt;&gt;" "),F23+G23,IF(AND(B23=" ",C23=" ")," ",G23))</f>
         <v>52363</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="31">
         <f>$B$6*(1000000-$B$9)*$B$14</f>
         <v>27750</v>
       </c>
       <c r="K23" s="14">
         <f>$B$5*E22</f>
-        <v>12950.000000000002</v>
+        <v>54950.000000000007</v>
       </c>
       <c r="L23" s="1">
         <f>SUM(H23:K23)</f>
-        <v>93063</v>
+        <v>135063</v>
       </c>
       <c r="P23" s="3"/>
     </row>
@@ -1342,7 +1249,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" ref="E24:E62" si="1">(E23-K24)*(1+D24)</f>
-        <v>370370.05434181727</v>
+        <v>1571570.2305855488</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ref="F24:F62" si="2">IF(AND(C24&lt;&gt;" ",C24&gt;$B$10),$B$11*(1+$B$16)^(A24-1),0)</f>
@@ -1362,11 +1269,11 @@
       </c>
       <c r="K24" s="14">
         <f t="shared" ref="K24:K52" si="4">$B$5*E23</f>
-        <v>12761.112333657475</v>
+        <v>54148.503686060096</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" ref="L24:L62" si="5">SUM(H24:K24)</f>
-        <v>69029.687333657464</v>
+        <v>110417.07868606009</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1386,7 +1293,7 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" si="1"/>
-        <v>396349.25613165606</v>
+        <v>1681806.303045135</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="2"/>
@@ -1406,11 +1313,11 @@
       </c>
       <c r="K25" s="14">
         <f t="shared" si="4"/>
-        <v>12962.951901963606</v>
+        <v>55004.958070494213</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="5"/>
-        <v>69944.491276963599</v>
+        <v>111986.4974454942</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="22" customFormat="1">
@@ -1430,7 +1337,7 @@
       </c>
       <c r="E26" s="24">
         <f t="shared" si="1"/>
-        <v>384991.93325366918</v>
+        <v>1633614.4194817855</v>
       </c>
       <c r="F26" s="24">
         <f t="shared" si="2"/>
@@ -1450,11 +1357,11 @@
       </c>
       <c r="K26" s="26">
         <f t="shared" si="4"/>
-        <v>13872.223964607963</v>
+        <v>58863.220606579729</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="5"/>
-        <v>71584.551823982969</v>
+        <v>116575.54846595472</v>
       </c>
       <c r="N26" s="24"/>
     </row>
@@ -1475,7 +1382,7 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" si="1"/>
-        <v>392169.43302607769</v>
+        <v>1664070.2968944379</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="2"/>
@@ -1495,11 +1402,11 @@
       </c>
       <c r="K27" s="14">
         <f t="shared" si="4"/>
-        <v>13474.717663878422</v>
+        <v>57176.504681862498</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="5"/>
-        <v>71936.103719737788</v>
+        <v>115637.89073772187</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1519,7 +1426,7 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" si="1"/>
-        <v>336413.29524558125</v>
+        <v>1427483.4419880069</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="2"/>
@@ -1539,11 +1446,11 @@
       </c>
       <c r="K28" s="14">
         <f t="shared" si="4"/>
-        <v>13725.93015591272</v>
+        <v>58242.460391305329</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="5"/>
-        <v>72955.100863168569</v>
+        <v>117471.63109856118</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1563,7 +1470,7 @@
       </c>
       <c r="E29" s="1">
         <f t="shared" si="1"/>
-        <v>381543.54750401032</v>
+        <v>1618982.0799494493</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="2"/>
@@ -1583,11 +1490,11 @@
       </c>
       <c r="K29" s="14">
         <f t="shared" si="4"/>
-        <v>11774.465333595344</v>
+        <v>49961.920469580247</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="5"/>
-        <v>71790.615308532593</v>
+        <v>109978.07044451749</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1607,7 +1514,7 @@
       </c>
       <c r="E30" s="1">
         <f t="shared" si="1"/>
-        <v>391584.94716009707</v>
+        <v>1661590.1811928446</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="2"/>
@@ -1627,11 +1534,11 @@
       </c>
       <c r="K30" s="14">
         <f t="shared" si="4"/>
-        <v>13354.024162640362</v>
+        <v>56664.372798230732</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="5"/>
-        <v>74176.82788695104</v>
+        <v>117487.17652254141</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1651,7 +1558,7 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" si="1"/>
-        <v>456518.61269007379</v>
+        <v>1937119.5187119353</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="2"/>
@@ -1671,11 +1578,11 @@
       </c>
       <c r="K31" s="14">
         <f t="shared" si="4"/>
-        <v>13705.473150603399</v>
+        <v>58155.656341749571</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="5"/>
-        <v>75355.09696802184</v>
+        <v>119805.280159168</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -1695,7 +1602,7 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" si="1"/>
-        <v>568699.85972731153</v>
+        <v>2413131.8372212956</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="2"/>
@@ -1715,11 +1622,11 @@
       </c>
       <c r="K32" s="14">
         <f t="shared" si="4"/>
-        <v>15978.151444152583</v>
+        <v>67799.183154917744</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="5"/>
-        <v>78475.265857006481</v>
+        <v>130296.29756777163</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -1739,7 +1646,7 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" si="1"/>
-        <v>556314.93295409402</v>
+        <v>2360579.5803727778</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="2"/>
@@ -1759,11 +1666,11 @@
       </c>
       <c r="K33" s="14">
         <f t="shared" si="4"/>
-        <v>19904.495090455905</v>
+        <v>84459.614302745351</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="5"/>
-        <v>83270.287363631141</v>
+        <v>147825.40657592058</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -1783,7 +1690,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" si="1"/>
-        <v>616280.74758729944</v>
+        <v>2615029.1181407035</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="2"/>
@@ -1803,11 +1710,11 @@
       </c>
       <c r="K34" s="14">
         <f t="shared" si="4"/>
-        <v>19471.022653393291</v>
+        <v>82620.285313047236</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="5"/>
-        <v>83727.209733397918</v>
+        <v>146876.47239305187</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1827,7 +1734,7 @@
       </c>
       <c r="E35" s="1">
         <f t="shared" si="1"/>
-        <v>604062.39978425787</v>
+        <v>2563183.6963818516</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="2"/>
@@ -1847,11 +1754,11 @@
       </c>
       <c r="K35" s="14">
         <f t="shared" si="4"/>
-        <v>21569.826165555482</v>
+        <v>91526.019134924631</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="5"/>
-        <v>86738.667922560213</v>
+        <v>156694.86089192936</v>
       </c>
       <c r="M35" t="s">
         <v>24</v>
@@ -1874,7 +1781,7 @@
       </c>
       <c r="E36" s="1">
         <f t="shared" si="1"/>
-        <v>668325.46837042063</v>
+        <v>2835867.5279501639</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="2"/>
@@ -1894,11 +1801,11 @@
       </c>
       <c r="K36" s="14">
         <f t="shared" si="4"/>
-        <v>21142.183992449027</v>
+        <v>89711.429373364808</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="5"/>
-        <v>87246.496793378872</v>
+        <v>155815.74217429466</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -1918,7 +1825,7 @@
       </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>707199.39816377219</v>
+        <v>3000819.0678841155</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="2"/>
@@ -1938,11 +1845,11 @@
       </c>
       <c r="K37" s="14">
         <f t="shared" si="4"/>
-        <v>23391.391392964724</v>
+        <v>99255.363478255749</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="5"/>
-        <v>90454.562013917821</v>
+        <v>166318.53409920883</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -1962,7 +1869,7 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>744366.30572698312</v>
+        <v>3158527.2972739567</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="2"/>
@@ -1982,11 +1889,11 @@
       </c>
       <c r="K38" s="14">
         <f t="shared" si="4"/>
-        <v>24751.97893573203</v>
+        <v>105028.66737594405</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="5"/>
-        <v>92797.978822208956</v>
+        <v>173074.66726242099</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2006,7 +1913,7 @@
       </c>
       <c r="E39" s="1">
         <f t="shared" si="1"/>
-        <v>620848.9593712606</v>
+        <v>2634413.1519267014</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="2"/>
@@ -2026,11 +1933,11 @@
       </c>
       <c r="K39" s="14">
         <f t="shared" si="4"/>
-        <v>26052.820700444412</v>
+        <v>110548.4554045885</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="5"/>
-        <v>95106.220584083261</v>
+        <v>179601.85528822735</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2050,7 +1957,7 @@
       </c>
       <c r="E40" s="1">
         <f t="shared" si="1"/>
-        <v>660693.64016742806</v>
+        <v>2803483.8244942226</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="2"/>
@@ -2070,11 +1977,11 @@
       </c>
       <c r="K40" s="14">
         <f t="shared" si="4"/>
-        <v>21729.713577994124</v>
+        <v>92204.460317434554</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="5"/>
-        <v>91815.698458723928</v>
+        <v>162290.44519816438</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2094,7 +2001,7 @@
       </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>588029.38887227257</v>
+        <v>2495151.731160725</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="2"/>
@@ -2118,11 +2025,11 @@
       </c>
       <c r="K41" s="14">
         <f t="shared" si="4"/>
-        <v>23124.277405859986</v>
+        <v>98121.933857297801</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="5"/>
-        <v>94268.661908608046</v>
+        <v>169266.31836004584</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2142,7 +2049,7 @@
       </c>
       <c r="E42" s="1">
         <f t="shared" si="1"/>
-        <v>746701.66472373507</v>
+        <v>3168436.7935574716</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="2"/>
@@ -2166,11 +2073,11 @@
       </c>
       <c r="K42" s="14">
         <f t="shared" si="4"/>
-        <v>20581.028610529542</v>
+        <v>87330.310590625377</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="5"/>
-        <v>92810.272725846298</v>
+        <v>159559.55470594214</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2190,7 +2097,7 @@
       </c>
       <c r="E43" s="1">
         <f t="shared" si="1"/>
-        <v>821343.34432104218</v>
+        <v>3485159.5961730718</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="2"/>
@@ -2214,11 +2121,11 @@
       </c>
       <c r="K43" s="14">
         <f t="shared" si="4"/>
-        <v>26134.558265330728</v>
+        <v>110895.28777451151</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="5"/>
-        <v>99475.783483530395</v>
+        <v>184236.51299271118</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2238,7 +2145,7 @@
       </c>
       <c r="E44" s="1">
         <f t="shared" si="1"/>
-        <v>1003709.8988104881</v>
+        <v>4258985.2463039644</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="2"/>
@@ -2262,11 +2169,11 @@
       </c>
       <c r="K44" s="14">
         <f t="shared" si="4"/>
-        <v>28747.017051236478</v>
+        <v>121980.58586605752</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="5"/>
-        <v>103228.02289989113</v>
+        <v>196461.59171471218</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="11" customFormat="1">
@@ -2286,7 +2193,7 @@
       </c>
       <c r="E45" s="12">
         <f t="shared" si="1"/>
-        <v>1021596.1783524178</v>
+        <v>4334881.0811170172</v>
       </c>
       <c r="F45" s="12">
         <f t="shared" si="2"/>
@@ -2310,11 +2217,11 @@
       </c>
       <c r="K45" s="30">
         <f t="shared" si="4"/>
-        <v>35129.846458367087</v>
+        <v>149064.48362063876</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="5"/>
-        <v>110779.12745323811</v>
+        <v>224713.76461550978</v>
       </c>
       <c r="N45" s="12"/>
     </row>
@@ -2335,7 +2242,7 @@
       </c>
       <c r="E46" s="12">
         <f t="shared" si="1"/>
-        <v>1116443.0195096128</v>
+        <v>4737339.2990002492</v>
       </c>
       <c r="F46" s="12">
         <f t="shared" si="2"/>
@@ -2359,11 +2266,11 @@
       </c>
       <c r="K46" s="30">
         <f t="shared" si="4"/>
-        <v>35755.866242334625</v>
+        <v>151720.83783909562</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="5"/>
-        <v>112602.62926207743</v>
+        <v>228567.60085883841</v>
       </c>
       <c r="N46" s="12"/>
     </row>
@@ -2384,7 +2291,7 @@
       </c>
       <c r="E47" s="12">
         <f t="shared" si="1"/>
-        <v>880056.22334106232</v>
+        <v>3734292.6233661301</v>
       </c>
       <c r="F47" s="12">
         <f t="shared" si="2"/>
@@ -2408,11 +2315,11 @@
       </c>
       <c r="K47" s="30">
         <f t="shared" si="4"/>
-        <v>39075.505682836454</v>
+        <v>165806.87546500875</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="5"/>
-        <v>117149.68777807284</v>
+        <v>243881.05756024513</v>
       </c>
       <c r="N47" s="12"/>
     </row>
@@ -2433,7 +2340,7 @@
       </c>
       <c r="E48" s="12">
         <f t="shared" si="1"/>
-        <v>709012.42305321631</v>
+        <v>3008512.1734960801</v>
       </c>
       <c r="F48" s="12">
         <f t="shared" si="2"/>
@@ -2457,11 +2364,11 @@
       </c>
       <c r="K48" s="30">
         <f t="shared" si="4"/>
-        <v>30801.967816937184</v>
+        <v>130700.24181781456</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="5"/>
-        <v>110134.25446455445</v>
+        <v>210032.52846543182</v>
       </c>
       <c r="N48" s="12"/>
     </row>
@@ -2482,7 +2389,7 @@
       </c>
       <c r="E49" s="12">
         <f t="shared" si="1"/>
-        <v>618823.73533747531</v>
+        <v>2625819.6337292874</v>
       </c>
       <c r="F49" s="12">
         <f t="shared" si="2"/>
@@ -2506,11 +2413,11 @@
       </c>
       <c r="K49" s="30">
         <f t="shared" si="4"/>
-        <v>24815.434806862573</v>
+        <v>105297.92607236281</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="5"/>
-        <v>105437.27862067027</v>
+        <v>185919.76988617051</v>
       </c>
       <c r="N49" s="12"/>
     </row>
@@ -2531,7 +2438,7 @@
       </c>
       <c r="E50" s="12">
         <f t="shared" si="1"/>
-        <v>705761.27675249078</v>
+        <v>2994716.7689227317</v>
       </c>
       <c r="F50" s="12">
         <f t="shared" si="2"/>
@@ -2555,11 +2462,11 @@
       </c>
       <c r="K50" s="30">
         <f t="shared" si="4"/>
-        <v>21658.830736811637</v>
+        <v>91903.68718052507</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" si="5"/>
-        <v>103602.47064596454</v>
+        <v>173847.32708967797</v>
       </c>
       <c r="N50" s="12"/>
     </row>
@@ -2580,7 +2487,7 @@
       </c>
       <c r="E51" s="12">
         <f t="shared" si="1"/>
-        <v>762574.93921580899</v>
+        <v>3235790.958294109</v>
       </c>
       <c r="F51" s="12">
         <f t="shared" si="2"/>
@@ -2604,11 +2511,11 @@
       </c>
       <c r="K51" s="30">
         <f t="shared" si="4"/>
-        <v>24701.644686337178</v>
+        <v>104815.08691229562</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="5"/>
-        <v>108000.12559321889</v>
+        <v>188113.56781917735</v>
       </c>
       <c r="N51" s="12"/>
     </row>
@@ -2629,7 +2536,7 @@
       </c>
       <c r="E52" s="12">
         <f t="shared" si="1"/>
-        <v>678179.15606206853</v>
+        <v>2877679.1216687774</v>
       </c>
       <c r="F52" s="12">
         <f t="shared" si="2"/>
@@ -2653,11 +2560,11 @@
       </c>
       <c r="K52" s="30">
         <f t="shared" si="4"/>
-        <v>26690.122872553318</v>
+        <v>113252.68354029383</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" si="5"/>
-        <v>111377.31580210707</v>
+        <v>197939.87646984757</v>
       </c>
       <c r="N52" s="12"/>
     </row>
@@ -2678,7 +2585,7 @@
       </c>
       <c r="E53" s="8">
         <f t="shared" si="1"/>
-        <v>815587.86548612651</v>
+        <v>3460737.6994951856</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="2"/>
@@ -2720,7 +2627,7 @@
       </c>
       <c r="E54" s="8">
         <f t="shared" si="1"/>
-        <v>910379.70457800932</v>
+        <v>3862962.5302364179</v>
       </c>
       <c r="F54" s="8">
         <f t="shared" si="2"/>
@@ -2762,7 +2669,7 @@
       </c>
       <c r="E55" s="8">
         <f t="shared" si="1"/>
-        <v>1025317.7273757438</v>
+        <v>4350672.5188646428</v>
       </c>
       <c r="F55" s="8">
         <f t="shared" si="2"/>
@@ -2804,7 +2711,7 @@
       </c>
       <c r="E56" s="8">
         <f t="shared" si="1"/>
-        <v>1161893.7441350259</v>
+        <v>4930197.7791675432</v>
       </c>
       <c r="F56" s="8">
         <f t="shared" si="2"/>
@@ -2846,7 +2753,7 @@
       </c>
       <c r="E57" s="8">
         <f t="shared" si="1"/>
-        <v>1304751.983373401</v>
+        <v>5536380.0375574054</v>
       </c>
       <c r="F57" s="8">
         <f t="shared" si="2"/>
@@ -2888,7 +2795,7 @@
       </c>
       <c r="E58" s="8">
         <f t="shared" si="1"/>
-        <v>1187757.541580213</v>
+        <v>5039944.1629214454</v>
       </c>
       <c r="F58" s="8">
         <f t="shared" si="2"/>
@@ -2930,7 +2837,7 @@
       </c>
       <c r="E59" s="8">
         <f t="shared" si="1"/>
-        <v>1006910.2349697308</v>
+        <v>4272565.0510877771</v>
       </c>
       <c r="F59" s="8">
         <f t="shared" si="2"/>
@@ -2972,7 +2879,7 @@
       </c>
       <c r="E60" s="8">
         <f t="shared" si="1"/>
-        <v>1034638.0548000487</v>
+        <v>4390220.9352326393</v>
       </c>
       <c r="F60" s="8">
         <f t="shared" si="2"/>
@@ -3014,7 +2921,7 @@
       </c>
       <c r="E61" s="8">
         <f t="shared" si="1"/>
-        <v>1100094.2628919571</v>
+        <v>4667967.5479469532</v>
       </c>
       <c r="F61" s="8">
         <f t="shared" si="2"/>
@@ -3056,7 +2963,7 @@
       </c>
       <c r="E62" s="8">
         <f t="shared" si="1"/>
-        <v>1114493.7251327834</v>
+        <v>4729067.9688066756</v>
       </c>
       <c r="F62" s="8">
         <f t="shared" si="2"/>

</xml_diff>